<commit_message>
Changelog of the Project
Last Change: Renamed project and removed directory structure
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob.Walker\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob.Walker\Documents\GitHub\Libre-Excel-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="Date_Updated">Sheet1!$B$9</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Libre Excel Tools for Data Science (LET4DataSci)</t>
-  </si>
-  <si>
-    <t>Let Forth Data Science!</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>ChangeLog</t>
   </si>
@@ -66,6 +57,18 @@
   </si>
   <si>
     <t>Initial work done to create LET4DataSci, created in a single file</t>
+  </si>
+  <si>
+    <t>Jacob@DataActionism.com</t>
+  </si>
+  <si>
+    <t>Libre Excel Tools</t>
+  </si>
+  <si>
+    <t>Let Forth Data!</t>
+  </si>
+  <si>
+    <t>Renaming of the project and removing directory structure</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -150,15 +153,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -166,9 +169,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -269,7 +275,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>LET4DataSci</a:t>
+            <a:t>Libre</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="800" baseline="0">
@@ -281,7 +287,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> is a collection of Libre (Open Source) tools to support doing data science and related work (BI, Machine Learning, etc.) with Excel.</a:t>
+            <a:t> Excel Tools are a collection of Libre (Open Source) tools to support doing a variety of work with data using Microsoft Excel</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="800"/>
         </a:p>
@@ -770,14 +776,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:F6" totalsRowShown="0">
-  <autoFilter ref="A5:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Change_Log" displayName="Change_Log" ref="A5:F7" totalsRowShown="0">
+  <autoFilter ref="A5:F7"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="1"/>
     <tableColumn id="2" name="Contributor"/>
     <tableColumn id="3" name="Email" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Version">
-      <calculatedColumnFormula>YEAR(Date_Updated)/10000+MONTH(Date_Updated)/1000000+DAY(Date_Updated)/100000000</calculatedColumnFormula>
+    <tableColumn id="4" name="Version" dataDxfId="0">
+      <calculatedColumnFormula>YEAR(Change_Log[[#This Row],[Date]])/10000+MONTH(Change_Log[[#This Row],[Date]])/1000000+DAY(Change_Log[[#This Row],[Date]])/100000000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Status"/>
     <tableColumn id="5" name="Major Changes"/>
@@ -1083,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1100,69 +1106,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.1" x14ac:dyDescent="0.85">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
+      <c r="A4" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>41674</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <f>YEAR(Change_Log[[#This Row],[Date]])/10000+MONTH(Change_Log[[#This Row],[Date]])/1000000+DAY(Change_Log[[#This Row],[Date]])/100000000</f>
+        <v>0.20140204</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
-        <f>YEAR(Date_Updated)/10000+MONTH(Date_Updated)/1000000+DAY(Date_Updated)/100000000</f>
-        <v>0.190001</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>43135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
+      <c r="D7">
+        <f>YEAR(Change_Log[[#This Row],[Date]])/10000+MONTH(Change_Log[[#This Row],[Date]])/1000000+DAY(Change_Log[[#This Row],[Date]])/100000000</f>
+        <v>0.20180204000000002</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1172,12 +1196,13 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>